<commit_message>
Added clear cache function
</commit_message>
<xml_diff>
--- a/public/listOfCities.xlsx
+++ b/public/listOfCities.xlsx
@@ -3122,7 +3122,7 @@
     <t xml:space="preserve">Шахтер</t>
   </si>
   <si>
-    <t xml:space="preserve">/shop_rostov.xls</t>
+    <t xml:space="preserve">/price_copy1.xls</t>
   </si>
 </sst>
 </file>
@@ -3362,7 +3362,7 @@
       <selection pane="bottomLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="100"/>
@@ -12713,10 +12713,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
@@ -12744,7 +12744,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>1032</v>
       </c>

</xml_diff>